<commit_message>
Till RAM of both Horizontal And Vertical
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/CreatePage.xlsx
+++ b/src/main/java/utilities/CreatePage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosh\Downloads\SSP\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A28B3F-BDD4-406D-9BB5-9333EE6DC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10AB7B5-B8A5-4D39-85EB-2403A2082586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{1BC5C445-E488-4687-9863-4BA2B5E53A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="11" xr2:uid="{1BC5C445-E488-4687-9863-4BA2B5E53A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,12 @@
     <sheet name="OSName" sheetId="4" r:id="rId4"/>
     <sheet name="IOPSValue" sheetId="5" r:id="rId5"/>
     <sheet name="LowerThresholdValue" sheetId="6" r:id="rId6"/>
+    <sheet name="UpperThresholdValue" sheetId="7" r:id="rId7"/>
+    <sheet name="VcpuValueForHScaling" sheetId="8" r:id="rId8"/>
+    <sheet name="VcpuvalueForVScaling" sheetId="9" r:id="rId9"/>
+    <sheet name="ToCheckAlert" sheetId="10" r:id="rId10"/>
+    <sheet name="RAMValueForHScaling" sheetId="11" r:id="rId11"/>
+    <sheet name="RAMValueForVScaling" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Sl.no</t>
   </si>
@@ -49,37 +55,79 @@
     <t>LocationName</t>
   </si>
   <si>
+    <t>AT_Testing</t>
+  </si>
+  <si>
+    <t>EC_Test_Linux_Storage_OCT_600 - 510GB</t>
+  </si>
+  <si>
+    <t>StoragePathName</t>
+  </si>
+  <si>
+    <t>OsName</t>
+  </si>
+  <si>
+    <t>Ubuntu 22.04 LTS (GUI)</t>
+  </si>
+  <si>
+    <t>IOPSValue</t>
+  </si>
+  <si>
+    <t>sl.no</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>LowerThresholdValue</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
     <t>Mysuru, India</t>
   </si>
   <si>
-    <t>AT_Testing</t>
-  </si>
-  <si>
-    <t>EC_Test_Linux_Storage_OCT_600 - 510GB</t>
-  </si>
-  <si>
-    <t>StoragePathName</t>
-  </si>
-  <si>
-    <t>OsName</t>
-  </si>
-  <si>
-    <t>Ubuntu 22.04 LTS (GUI)</t>
-  </si>
-  <si>
-    <t>IOPSValue</t>
-  </si>
-  <si>
-    <t>sl.no</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>LowerThresholdValue</t>
-  </si>
-  <si>
-    <t>40</t>
+    <t>80</t>
+  </si>
+  <si>
+    <t>UpperThresholdValue</t>
+  </si>
+  <si>
+    <t>VcpuValueForHScaling</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>MaxVcpuValueForVScaling</t>
+  </si>
+  <si>
+    <t>MinVcpuValueForVScaling</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Sl.no(min value should be greater than max value)</t>
+  </si>
+  <si>
+    <t>RamValueForHScaling</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>MaxRAMValueForVScaling</t>
+  </si>
+  <si>
+    <t>MinRAMValueForVScaling</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -455,7 +503,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +521,112 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1879196D-E013-466F-ADC7-4D53087CC28E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C62C852-3CDB-4B2C-A3FC-784E04168D79}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBAD17F-6E9D-4AF4-A460-C61C14849213}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -504,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -559,21 +712,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -593,18 +746,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -616,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3383406-9E87-4B18-86AC-E8D9ADAF63BA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,19 +780,118 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CCF50B-54F6-4A47-9D57-0CD3D0CB6D5F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79862244-3E74-4181-AEEC-C1056025484B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E958E3C9-9E68-4C55-B3ED-086087EB51FB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All Cases DOne in Create Page
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/CreatePage.xlsx
+++ b/src/main/java/utilities/CreatePage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosh\Downloads\SSP\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B6B6C5-1871-4E81-8A9A-2771FB5FE646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFF0AB8-89C6-491B-94A5-3D13C29FB2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="17" activeTab="20" xr2:uid="{1BC5C445-E488-4687-9863-4BA2B5E53A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="22" xr2:uid="{1BC5C445-E488-4687-9863-4BA2B5E53A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,10 @@
     <sheet name="RetentionPeriodValue" sheetId="19" r:id="rId19"/>
     <sheet name="SIEMName" sheetId="20" r:id="rId20"/>
     <sheet name="VLANName" sheetId="21" r:id="rId21"/>
+    <sheet name="NumberOfVms" sheetId="22" r:id="rId22"/>
+    <sheet name="VMNamesForH" sheetId="23" r:id="rId23"/>
+    <sheet name="VMNamesForV" sheetId="24" r:id="rId24"/>
+    <sheet name="UserInfo" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>Sl.no</t>
   </si>
@@ -67,33 +71,21 @@
     <t>AT_Testing</t>
   </si>
   <si>
-    <t>EC_Test_Linux_Storage_OCT_600 - 510GB</t>
-  </si>
-  <si>
     <t>StoragePathName</t>
   </si>
   <si>
     <t>OsName</t>
   </si>
   <si>
-    <t>Ubuntu 22.04 LTS (GUI)</t>
-  </si>
-  <si>
     <t>IOPSValue</t>
   </si>
   <si>
     <t>sl.no</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>LowerThresholdValue</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>Mysuru, India</t>
   </si>
   <si>
@@ -103,9 +95,6 @@
     <t>VcpuValueForHScaling</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>MaxVcpuValueForVScaling</t>
   </si>
   <si>
@@ -163,12 +152,6 @@
     <t>RetentionPeriodValue</t>
   </si>
   <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>12 months</t>
-  </si>
-  <si>
     <t>SIEMName</t>
   </si>
   <si>
@@ -178,7 +161,79 @@
     <t>VlanName</t>
   </si>
   <si>
-    <t>10.150.35.0 - akashTest</t>
+    <t>10.150.36.0 - teshtshweta</t>
+  </si>
+  <si>
+    <t>SL.no</t>
+  </si>
+  <si>
+    <t>NumberOFVMs</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>VMNamesfor H</t>
+  </si>
+  <si>
+    <t>VMNamesforV</t>
+  </si>
+  <si>
+    <t>No.OfVms</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>SelectAllCondition</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>karthik</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>lead2</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>Storage_Linux_Sep17 - 768GB</t>
+  </si>
+  <si>
+    <t>CentOS Stream 8 (CLI)</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
   </si>
 </sst>
 </file>
@@ -572,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +640,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,10 +650,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,10 +661,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -629,13 +684,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -669,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +745,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +755,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,10 +766,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -727,17 +782,17 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -796,13 +851,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,10 +865,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -836,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -898,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -906,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -961,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -969,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -981,6 +1036,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B60CDD4-3C4A-4D3C-8FAA-5F42A54BD336}">
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181AE484-7116-431E-88ED-89D201FEF9D7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD16252E-7D14-43B4-A47A-854697887676}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -992,15 +1109,109 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF61A9B-456C-475F-A236-E0D2C5F0AF55}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39ABDC7-88EE-4A76-8F80-3B0DE47D6046}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1031,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +1265,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1065,10 +1276,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1081,17 +1292,17 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1099,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1122,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1130,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1193,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1205,18 +1416,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79862244-3E74-4181-AEEC-C1056025484B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1224,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on Storage page
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/CreatePage.xlsx
+++ b/src/main/java/utilities/CreatePage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosh\Downloads\SSP\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2474ECD5-2D72-4052-928B-C6C214C5ABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C90618C-F6F3-4B2F-A91F-106AEB9D5FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="20" activeTab="22" xr2:uid="{1BC5C445-E488-4687-9863-4BA2B5E53A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{1BC5C445-E488-4687-9863-4BA2B5E53A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>lead2</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -221,25 +218,28 @@
     <t>3 days</t>
   </si>
   <si>
-    <t>lead3</t>
-  </si>
-  <si>
     <t>Ubuntu 22.04 LTS (CLI)</t>
   </si>
   <si>
-    <t>Storage_Linux_Sep17 - 850GB</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>10.150.37.0 - karthik</t>
-  </si>
-  <si>
     <t>test7,test8,test9</t>
   </si>
   <si>
     <t>test1</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>10.150.43.0 - Test_01</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Storage3_2025 - 122GB</t>
   </si>
 </sst>
 </file>
@@ -667,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -772,10 +772,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD16252E-7D14-43B4-A47A-854697887676}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1124,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1158,10 +1158,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39ABDC7-88EE-4A76-8F80-3B0DE47D6046}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,10 +1215,10 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
         <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -1263,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733DF0AA-013B-4F7D-BB8E-6161E95F980B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1298,10 +1298,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1457,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>